<commit_message>
Added Extent Report code and few Modification
</commit_message>
<xml_diff>
--- a/src/test/resources/app/Amazon_data.xlsx
+++ b/src/test/resources/app/Amazon_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spaunikar/Documents/Cognizant_test_demo/src/test/resources/app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spaunikar/Documents/NewWiproDemo/AmazonTest/src/test/resources/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CEF6E3-8E76-8945-92C3-4F09BEF21BD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F5679C-90DA-064A-BB71-A648691011B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16160" xr2:uid="{ACDC20F4-750A-4645-86AC-53E5A0324ABB}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16080" xr2:uid="{ACDC20F4-750A-4645-86AC-53E5A0324ABB}"/>
   </bookViews>
   <sheets>
     <sheet name="itemSheet" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Item_name</t>
   </si>
   <si>
     <t>65-inch TV</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -397,21 +409,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21742613-810D-1142-AAFA-1206679BD7F9}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>